<commit_message>
Enclosure DWG & BOMs
</commit_message>
<xml_diff>
--- a/docs/Kicad Files/Amplifier/Power_Amp_RevB/BOM/Power_Amp_RevB.xlsx
+++ b/docs/Kicad Files/Amplifier/Power_Amp_RevB/BOM/Power_Amp_RevB.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/85ce5863630a9cf8/Documents/15-Fall 2024/EE 492/Bluetooth-Speaker-Senior-Design/docs/Kicad Files/Amplifier/Power_Amp_RevB/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{373B66E4-E4D0-4628-8BC5-924D0B379AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56D1FD8A-F7F1-4EA5-AA58-662B7A36326B}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{373B66E4-E4D0-4628-8BC5-924D0B379AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6792814-391B-4DA8-AF1D-9BF40234738B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{513FAEA2-BE9C-48BA-8BBE-55C685E2CB0C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{513FAEA2-BE9C-48BA-8BBE-55C685E2CB0C}"/>
   </bookViews>
   <sheets>
     <sheet name="Power_Amp_RevB" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>Reference</t>
   </si>
@@ -37,18 +38,12 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
     <t>C1,C7</t>
   </si>
   <si>
     <t>0.22Uf</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
     <t>Capacitor_THT:C_Rect_L7.0mm_W3.5mm_P5.00mm</t>
   </si>
   <si>
@@ -187,24 +182,9 @@
     <t>Potentiometer_THT:Potentiometer_Bourns_3386P_Vertical</t>
   </si>
   <si>
-    <t>TP1,TP2</t>
-  </si>
-  <si>
-    <t>TestPoint</t>
-  </si>
-  <si>
-    <t>TestPoint:TestPoint_THTPad_D2.0mm_Drill1.0mm</t>
-  </si>
-  <si>
-    <t>https://www.nichicon.co.jp/english/series_items/catalog_pdf/e-uvr.pdf</t>
-  </si>
-  <si>
     <t>https://search.kemet.com/download/datasheet/ESK105M050AC3AA</t>
   </si>
   <si>
-    <t>https://www.cde.com/resources/catalogs/CD-CDV16.pdf</t>
-  </si>
-  <si>
     <t>https://industrial.panasonic.com/cdbs/www-data/pdf/RDF0000/ABA0000C1215.pdf</t>
   </si>
   <si>
@@ -218,13 +198,73 @@
   </si>
   <si>
     <t>https://www.ttelectronics.com/TTElectronics/media/ProductFiles/Datasheet/P090.pdf</t>
+  </si>
+  <si>
+    <t>https://www.cde.com/resources/catalogs/STD-DIPPED.pdf</t>
+  </si>
+  <si>
+    <t>P/N</t>
+  </si>
+  <si>
+    <t>CD15FD221JO3</t>
+  </si>
+  <si>
+    <t>ESK105M050AC3AA</t>
+  </si>
+  <si>
+    <t>CF18JT4K70</t>
+  </si>
+  <si>
+    <t>CDV19FF102JO3F</t>
+  </si>
+  <si>
+    <t>ECA-0JHG102</t>
+  </si>
+  <si>
+    <t>CF14JT10K0</t>
+  </si>
+  <si>
+    <t>MFR-25FTF52-0R22</t>
+  </si>
+  <si>
+    <t>CF14JT12K0</t>
+  </si>
+  <si>
+    <t>CF14JT1K30</t>
+  </si>
+  <si>
+    <t>P090S-04F20BR10K</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>Screw Terminal</t>
+  </si>
+  <si>
+    <t>Transistor</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Power Amplifier Board BOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,6 +407,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -549,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -664,6 +712,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -710,10 +773,18 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -773,6 +844,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,384 +1167,492 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36C4C1F-8F92-4F6B-A7F6-554E2417F6C2}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="72.6328125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="5">
+        <v>691137710002</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="5">
+        <v>691137710002</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="5">
+        <v>691137710002</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G17" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
+      <c r="E20" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.22</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{8480BC43-0336-4964-8AC8-F69DA67C00E2}"/>
-    <hyperlink ref="C6" r:id="rId2" xr:uid="{43D68EA2-5DF7-4A40-81C3-C6FB6F3A98B8}"/>
-    <hyperlink ref="C10" r:id="rId3" xr:uid="{219A69C5-7279-424A-8141-ECB347CBF2EE}"/>
-    <hyperlink ref="C11" r:id="rId4" xr:uid="{1364C450-335C-47BC-8778-3E0B53781291}"/>
-    <hyperlink ref="C12" r:id="rId5" xr:uid="{429FD73B-09F5-4A7E-A77F-09748AD4B6FA}"/>
-    <hyperlink ref="C13" r:id="rId6" xr:uid="{73A0001D-6D76-4270-A646-7073BF1DF168}"/>
-    <hyperlink ref="C3" r:id="rId7" xr:uid="{6B6924E1-923D-45C3-BA3A-5B4C9671E87C}"/>
-    <hyperlink ref="C4" r:id="rId8" xr:uid="{79DFEDEE-81EA-403C-8509-8BCCCEADAF2C}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{ED2804F7-1CEA-4510-A17E-AE82C725DF65}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{2B1D29E6-532A-4DAB-B508-B52EF71BD1A9}"/>
-    <hyperlink ref="C8:C9" r:id="rId11" display="https://www.we-online.com/katalog/datasheet/691137710002.pdf" xr:uid="{748FF2DF-D9F7-4DB7-8406-499DF0296E40}"/>
-    <hyperlink ref="C14" r:id="rId12" xr:uid="{6FF3BFA3-D969-484B-BE8E-2EB04A92471D}"/>
-    <hyperlink ref="C15" r:id="rId13" xr:uid="{A8974C78-5E0E-4D0F-8A45-2C714A146E85}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{8C5B8FE7-F349-45F2-BBEF-3D6AC2405C2E}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{E0075F9A-3ABD-4F57-A197-80257ED6273D}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{56E85010-76C4-4233-809A-F7EF69344159}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{924AE1B3-80E0-4931-8E5B-1D9C684E86B0}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{8480BC43-0336-4964-8AC8-F69DA67C00E2}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{43D68EA2-5DF7-4A40-81C3-C6FB6F3A98B8}"/>
+    <hyperlink ref="D11" r:id="rId3" xr:uid="{219A69C5-7279-424A-8141-ECB347CBF2EE}"/>
+    <hyperlink ref="D12" r:id="rId4" xr:uid="{1364C450-335C-47BC-8778-3E0B53781291}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{429FD73B-09F5-4A7E-A77F-09748AD4B6FA}"/>
+    <hyperlink ref="D14" r:id="rId6" xr:uid="{73A0001D-6D76-4270-A646-7073BF1DF168}"/>
+    <hyperlink ref="D4" r:id="rId7" xr:uid="{6B6924E1-923D-45C3-BA3A-5B4C9671E87C}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{79DFEDEE-81EA-403C-8509-8BCCCEADAF2C}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{ED2804F7-1CEA-4510-A17E-AE82C725DF65}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{2B1D29E6-532A-4DAB-B508-B52EF71BD1A9}"/>
+    <hyperlink ref="D9:D10" r:id="rId11" display="https://www.we-online.com/katalog/datasheet/691137710002.pdf" xr:uid="{748FF2DF-D9F7-4DB7-8406-499DF0296E40}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{6FF3BFA3-D969-484B-BE8E-2EB04A92471D}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{A8974C78-5E0E-4D0F-8A45-2C714A146E85}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{8C5B8FE7-F349-45F2-BBEF-3D6AC2405C2E}"/>
+    <hyperlink ref="D18" r:id="rId15" xr:uid="{E0075F9A-3ABD-4F57-A197-80257ED6273D}"/>
+    <hyperlink ref="D19" r:id="rId16" xr:uid="{56E85010-76C4-4233-809A-F7EF69344159}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{924AE1B3-80E0-4931-8E5B-1D9C684E86B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>